<commit_message>
add ui for script
</commit_message>
<xml_diff>
--- a/Examples/export.xlsx
+++ b/Examples/export.xlsx
@@ -419,7 +419,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -439,7 +439,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -459,7 +459,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
made export work globally for all tables
</commit_message>
<xml_diff>
--- a/Examples/export.xlsx
+++ b/Examples/export.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -41,16 +41,22 @@
     <t>abcd</t>
   </si>
   <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>ijkl</t>
+  </si>
+  <si>
     <t>test2</t>
   </si>
   <si>
     <t>efgh</t>
   </si>
   <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>ijkl</t>
+    <t>dsf</t>
+  </si>
+  <si>
+    <t>sefse</t>
   </si>
 </sst>
 </file>
@@ -389,7 +395,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,7 +445,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -448,7 +454,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -459,7 +465,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -468,12 +474,52 @@
         <v>11</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
     </row>

</xml_diff>